<commit_message>
Ajout de plusieurs liste de questions
</commit_message>
<xml_diff>
--- a/data/Amenagement_urbain_durable.xlsx
+++ b/data/Amenagement_urbain_durable.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Mono</t>
   </si>
   <si>
-    <t xml:space="preserve">q2</t>
+    <t xml:space="preserve">8a</t>
   </si>
   <si>
     <t xml:space="preserve">Un syndicat mixte</t>
@@ -71,7 +71,10 @@
     <t xml:space="preserve">o</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1</t>
+    <t xml:space="preserve">8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8;q8a</t>
   </si>
   <si>
     <t xml:space="preserve">Oui</t>
@@ -89,7 +92,7 @@
     <t xml:space="preserve">Multichoix</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2</t>
+    <t xml:space="preserve">8.2</t>
   </si>
   <si>
     <t xml:space="preserve">PROJET</t>
@@ -136,11 +139,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,17 +170,13 @@
     <font>
       <sz val="9"/>
       <name val="Calibri Light"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri Light"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
     </font>
@@ -235,35 +235,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,9 +290,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2539800</xdr:colOff>
+      <xdr:colOff>2539080</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -302,9 +302,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="6995880" y="11799720"/>
-          <a:ext cx="397800" cy="322200"/>
+          <a:ext cx="397080" cy="321480"/>
           <a:chOff x="6995880" y="11799720"/>
-          <a:chExt cx="397800" cy="322200"/>
+          <a:chExt cx="397080" cy="321480"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -315,13 +315,18 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="6995880" y="11799720"/>
-            <a:ext cx="397800" cy="322200"/>
+            <a:ext cx="397080" cy="321480"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
-            <a:gdLst/>
+            <a:gdLst>
+              <a:gd name="textAreaLeft" fmla="*/ 0 w 397080"/>
+              <a:gd name="textAreaRight" fmla="*/ 397800 w 397080"/>
+              <a:gd name="textAreaTop" fmla="*/ 0 h 321480"/>
+              <a:gd name="textAreaBottom" fmla="*/ 322200 h 321480"/>
+            </a:gdLst>
             <a:ahLst/>
-            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
             <a:pathLst>
               <a:path w="398145" h="322580">
                 <a:moveTo>
@@ -374,7 +379,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="6995880" y="11799720"/>
-            <a:ext cx="397800" cy="322200"/>
+            <a:ext cx="397080" cy="321480"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -402,8 +407,12 @@
             </a:pPr>
             <a:r>
               <a:rPr b="1" lang="fr-FR" sz="1300" strike="noStrike" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
               <a:t>6</a:t>
             </a:r>
@@ -534,56 +543,56 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="63.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -592,24 +601,24 @@
       <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -618,246 +627,246 @@
       <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="D8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="H8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>2</v>
+      <c r="A10" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>3</v>
+      <c r="A13" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J17" s="2"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J19" s="2"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J20" s="2"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>